<commit_message>
Updating Position Paper Figures
</commit_message>
<xml_diff>
--- a/Data/BMI_Obese_Data.xlsx
+++ b/Data/BMI_Obese_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/reuben_frost_icr_ac_uk/Documents/Documents/UK-cancer-trends/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{5F7CB2F2-6FCA-4E46-93D7-A408BDB3CA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B66414AB-8A91-45B3-BB72-D9DF9D2712D3}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{5F7CB2F2-6FCA-4E46-93D7-A408BDB3CA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D0BB13B-1C7B-4086-95EB-1684B3A9961C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{829D32ED-C335-430B-9CDD-9FA1FEF3E92C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{829D32ED-C335-430B-9CDD-9FA1FEF3E92C}"/>
   </bookViews>
   <sheets>
     <sheet name="Scotland_Sex" sheetId="4" r:id="rId1"/>
@@ -1062,16 +1062,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1694D13A-39AC-4F8C-A50A-6BD751D42DE3}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:J85"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1103,7 +1102,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2008</v>
       </c>
@@ -1135,7 +1134,7 @@
         <v>5477</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2008</v>
       </c>
@@ -1167,7 +1166,7 @@
         <v>5477</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2008</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>3020</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2008</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>3020</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2008</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2008</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2009</v>
       </c>
@@ -1327,7 +1326,7 @@
         <v>6299</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2009</v>
       </c>
@@ -1359,7 +1358,7 @@
         <v>6299</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2009</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -1423,7 +1422,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2009</v>
       </c>
@@ -1455,7 +1454,7 @@
         <v>2843</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2009</v>
       </c>
@@ -1487,7 +1486,7 @@
         <v>2843</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2010</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>6001</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2010</v>
       </c>
@@ -1551,7 +1550,7 @@
         <v>6001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2010</v>
       </c>
@@ -1583,7 +1582,7 @@
         <v>3327</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2010</v>
       </c>
@@ -1615,7 +1614,7 @@
         <v>3327</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2010</v>
       </c>
@@ -1647,7 +1646,7 @@
         <v>2674</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2010</v>
       </c>
@@ -1679,7 +1678,7 @@
         <v>2674</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2011</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>6134</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2011</v>
       </c>
@@ -1743,7 +1742,7 @@
         <v>6134</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2011</v>
       </c>
@@ -1775,7 +1774,7 @@
         <v>3389</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>3389</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -1839,7 +1838,7 @@
         <v>2745</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2011</v>
       </c>
@@ -1871,7 +1870,7 @@
         <v>2745</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2012</v>
       </c>
@@ -1903,7 +1902,7 @@
         <v>4097</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2012</v>
       </c>
@@ -1935,7 +1934,7 @@
         <v>4097</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2012</v>
       </c>
@@ -1967,7 +1966,7 @@
         <v>2221</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2012</v>
       </c>
@@ -1999,7 +1998,7 @@
         <v>2221</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2012</v>
       </c>
@@ -2031,7 +2030,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2012</v>
       </c>
@@ -2063,7 +2062,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2013</v>
       </c>
@@ -2095,7 +2094,7 @@
         <v>4132</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2013</v>
       </c>
@@ -2127,7 +2126,7 @@
         <v>4132</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2013</v>
       </c>
@@ -2159,7 +2158,7 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2013</v>
       </c>
@@ -2191,7 +2190,7 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2013</v>
       </c>
@@ -2223,7 +2222,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2013</v>
       </c>
@@ -2255,7 +2254,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2014</v>
       </c>
@@ -2287,7 +2286,7 @@
         <v>3969</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2014</v>
       </c>
@@ -2319,7 +2318,7 @@
         <v>3969</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2014</v>
       </c>
@@ -2351,7 +2350,7 @@
         <v>2198</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2014</v>
       </c>
@@ -2383,7 +2382,7 @@
         <v>2198</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2014</v>
       </c>
@@ -2415,7 +2414,7 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2014</v>
       </c>
@@ -2447,7 +2446,7 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2015</v>
       </c>
@@ -2479,7 +2478,7 @@
         <v>4050</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2015</v>
       </c>
@@ -2511,7 +2510,7 @@
         <v>4050</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2015</v>
       </c>
@@ -2543,7 +2542,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2015</v>
       </c>
@@ -2575,7 +2574,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2015</v>
       </c>
@@ -2607,7 +2606,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2015</v>
       </c>
@@ -2639,7 +2638,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2016</v>
       </c>
@@ -2671,7 +2670,7 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2016</v>
       </c>
@@ -2703,7 +2702,7 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2016</v>
       </c>
@@ -2735,7 +2734,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2016</v>
       </c>
@@ -2767,7 +2766,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2016</v>
       </c>
@@ -2799,7 +2798,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2016</v>
       </c>
@@ -2831,7 +2830,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2017</v>
       </c>
@@ -2863,7 +2862,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2017</v>
       </c>
@@ -2895,7 +2894,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2017</v>
       </c>
@@ -2927,7 +2926,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2017</v>
       </c>
@@ -2959,7 +2958,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2017</v>
       </c>
@@ -2991,7 +2990,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2017</v>
       </c>
@@ -3023,7 +3022,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2018</v>
       </c>
@@ -3055,7 +3054,7 @@
         <v>3725</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2018</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>3725</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>2018</v>
       </c>
@@ -3119,7 +3118,7 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>2018</v>
       </c>
@@ -3151,7 +3150,7 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>2018</v>
       </c>
@@ -3183,7 +3182,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>2018</v>
       </c>
@@ -3215,7 +3214,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>2019</v>
       </c>
@@ -3247,7 +3246,7 @@
         <v>3889</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>2019</v>
       </c>
@@ -3279,7 +3278,7 @@
         <v>3889</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>2019</v>
       </c>
@@ -3311,7 +3310,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>2019</v>
       </c>
@@ -3343,7 +3342,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>2019</v>
       </c>
@@ -3375,7 +3374,7 @@
         <v>1759</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>2019</v>
       </c>
@@ -3407,7 +3406,7 @@
         <v>1759</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>2021</v>
       </c>
@@ -3439,7 +3438,7 @@
         <v>4122</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>2021</v>
       </c>
@@ -3471,7 +3470,7 @@
         <v>4122</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2021</v>
       </c>
@@ -3503,7 +3502,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>2021</v>
       </c>
@@ -3535,7 +3534,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>2021</v>
       </c>
@@ -3567,7 +3566,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>2021</v>
       </c>
@@ -3599,7 +3598,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>2022</v>
       </c>
@@ -3631,7 +3630,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>2022</v>
       </c>
@@ -3663,7 +3662,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>2022</v>
       </c>
@@ -3695,7 +3694,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>2022</v>
       </c>
@@ -3727,7 +3726,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>2022</v>
       </c>
@@ -3759,7 +3758,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>2022</v>
       </c>
@@ -3792,13 +3791,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J85" xr:uid="{1694D13A-39AC-4F8C-A50A-6BD751D42DE3}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Obesity"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3811,9 +3803,9 @@
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3845,7 +3837,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2008</v>
       </c>
@@ -3877,7 +3869,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2008</v>
       </c>
@@ -3909,7 +3901,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2008</v>
       </c>
@@ -3941,7 +3933,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2008</v>
       </c>
@@ -3973,7 +3965,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2008</v>
       </c>
@@ -4005,7 +3997,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2008</v>
       </c>
@@ -4037,7 +4029,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2008</v>
       </c>
@@ -4069,7 +4061,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2008</v>
       </c>
@@ -4101,7 +4093,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -4133,7 +4125,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2008</v>
       </c>
@@ -4165,7 +4157,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2008</v>
       </c>
@@ -4197,7 +4189,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2008</v>
       </c>
@@ -4229,7 +4221,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2008</v>
       </c>
@@ -4261,7 +4253,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2008</v>
       </c>
@@ -4293,7 +4285,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2008</v>
       </c>
@@ -4325,7 +4317,7 @@
         <v>5477</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2008</v>
       </c>
@@ -4357,7 +4349,7 @@
         <v>5477</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2009</v>
       </c>
@@ -4389,7 +4381,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2009</v>
       </c>
@@ -4421,7 +4413,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2009</v>
       </c>
@@ -4453,7 +4445,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2009</v>
       </c>
@@ -4485,7 +4477,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2009</v>
       </c>
@@ -4517,7 +4509,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2009</v>
       </c>
@@ -4549,7 +4541,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2009</v>
       </c>
@@ -4581,7 +4573,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2009</v>
       </c>
@@ -4613,7 +4605,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2009</v>
       </c>
@@ -4645,7 +4637,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2009</v>
       </c>
@@ -4677,7 +4669,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2009</v>
       </c>
@@ -4709,7 +4701,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2009</v>
       </c>
@@ -4741,7 +4733,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2009</v>
       </c>
@@ -4773,7 +4765,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2009</v>
       </c>
@@ -4805,7 +4797,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2009</v>
       </c>
@@ -4837,7 +4829,7 @@
         <v>6299</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2009</v>
       </c>
@@ -4869,7 +4861,7 @@
         <v>6299</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2010</v>
       </c>
@@ -4901,7 +4893,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2010</v>
       </c>
@@ -4933,7 +4925,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2010</v>
       </c>
@@ -4965,7 +4957,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2010</v>
       </c>
@@ -4997,7 +4989,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2010</v>
       </c>
@@ -5029,7 +5021,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2010</v>
       </c>
@@ -5061,7 +5053,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2010</v>
       </c>
@@ -5093,7 +5085,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2010</v>
       </c>
@@ -5125,7 +5117,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2010</v>
       </c>
@@ -5157,7 +5149,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2010</v>
       </c>
@@ -5189,7 +5181,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2010</v>
       </c>
@@ -5221,7 +5213,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2010</v>
       </c>
@@ -5253,7 +5245,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2010</v>
       </c>
@@ -5285,7 +5277,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2010</v>
       </c>
@@ -5317,7 +5309,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2010</v>
       </c>
@@ -5349,7 +5341,7 @@
         <v>6001</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2010</v>
       </c>
@@ -5381,7 +5373,7 @@
         <v>6001</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2011</v>
       </c>
@@ -5413,7 +5405,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2011</v>
       </c>
@@ -5445,7 +5437,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2011</v>
       </c>
@@ -5477,7 +5469,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2011</v>
       </c>
@@ -5509,7 +5501,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2011</v>
       </c>
@@ -5541,7 +5533,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2011</v>
       </c>
@@ -5573,7 +5565,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2011</v>
       </c>
@@ -5605,7 +5597,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2011</v>
       </c>
@@ -5637,7 +5629,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2011</v>
       </c>
@@ -5669,7 +5661,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2011</v>
       </c>
@@ -5701,7 +5693,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2011</v>
       </c>
@@ -5733,7 +5725,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2011</v>
       </c>
@@ -5765,7 +5757,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2011</v>
       </c>
@@ -5797,7 +5789,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2011</v>
       </c>
@@ -5829,7 +5821,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>2011</v>
       </c>
@@ -5861,7 +5853,7 @@
         <v>6134</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>2011</v>
       </c>
@@ -5893,7 +5885,7 @@
         <v>6134</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>2012</v>
       </c>
@@ -5925,7 +5917,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>2012</v>
       </c>
@@ -5957,7 +5949,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>2012</v>
       </c>
@@ -5989,7 +5981,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>2012</v>
       </c>
@@ -6021,7 +6013,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>2012</v>
       </c>
@@ -6053,7 +6045,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>2012</v>
       </c>
@@ -6085,7 +6077,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>2012</v>
       </c>
@@ -6117,7 +6109,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>2012</v>
       </c>
@@ -6149,7 +6141,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>2012</v>
       </c>
@@ -6181,7 +6173,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>2012</v>
       </c>
@@ -6213,7 +6205,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2012</v>
       </c>
@@ -6245,7 +6237,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>2012</v>
       </c>
@@ -6277,7 +6269,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>2012</v>
       </c>
@@ -6309,7 +6301,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>2012</v>
       </c>
@@ -6341,7 +6333,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>2012</v>
       </c>
@@ -6373,7 +6365,7 @@
         <v>4097</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>2012</v>
       </c>
@@ -6405,7 +6397,7 @@
         <v>4097</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>2013</v>
       </c>
@@ -6437,7 +6429,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>2013</v>
       </c>
@@ -6469,7 +6461,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>2013</v>
       </c>
@@ -6501,7 +6493,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>2013</v>
       </c>
@@ -6533,7 +6525,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>2013</v>
       </c>
@@ -6565,7 +6557,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>2013</v>
       </c>
@@ -6597,7 +6589,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>2013</v>
       </c>
@@ -6629,7 +6621,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>2013</v>
       </c>
@@ -6661,7 +6653,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>2013</v>
       </c>
@@ -6693,7 +6685,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>2013</v>
       </c>
@@ -6725,7 +6717,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>2013</v>
       </c>
@@ -6757,7 +6749,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>2013</v>
       </c>
@@ -6789,7 +6781,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>2013</v>
       </c>
@@ -6821,7 +6813,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>2013</v>
       </c>
@@ -6853,7 +6845,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>2013</v>
       </c>
@@ -6885,7 +6877,7 @@
         <v>4132</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>2013</v>
       </c>
@@ -6917,7 +6909,7 @@
         <v>4132</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>2014</v>
       </c>
@@ -6949,7 +6941,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>2014</v>
       </c>
@@ -6981,7 +6973,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>2014</v>
       </c>
@@ -7013,7 +7005,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>2014</v>
       </c>
@@ -7045,7 +7037,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>2014</v>
       </c>
@@ -7077,7 +7069,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>2014</v>
       </c>
@@ -7109,7 +7101,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -7141,7 +7133,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>2014</v>
       </c>
@@ -7173,7 +7165,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>2014</v>
       </c>
@@ -7205,7 +7197,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>2014</v>
       </c>
@@ -7237,7 +7229,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -7269,7 +7261,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>2014</v>
       </c>
@@ -7301,7 +7293,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>2014</v>
       </c>
@@ -7333,7 +7325,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>2014</v>
       </c>
@@ -7365,7 +7357,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -7397,7 +7389,7 @@
         <v>3969</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>2014</v>
       </c>
@@ -7429,7 +7421,7 @@
         <v>3969</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>2015</v>
       </c>
@@ -7461,7 +7453,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>2015</v>
       </c>
@@ -7493,7 +7485,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>2015</v>
       </c>
@@ -7525,7 +7517,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>2015</v>
       </c>
@@ -7557,7 +7549,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>2015</v>
       </c>
@@ -7589,7 +7581,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>2015</v>
       </c>
@@ -7621,7 +7613,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>2015</v>
       </c>
@@ -7653,7 +7645,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -7685,7 +7677,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>2015</v>
       </c>
@@ -7717,7 +7709,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>2015</v>
       </c>
@@ -7749,7 +7741,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>2015</v>
       </c>
@@ -7781,7 +7773,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>2015</v>
       </c>
@@ -7813,7 +7805,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>2015</v>
       </c>
@@ -7845,7 +7837,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>2015</v>
       </c>
@@ -7877,7 +7869,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>2015</v>
       </c>
@@ -7909,7 +7901,7 @@
         <v>4050</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>2015</v>
       </c>
@@ -7941,7 +7933,7 @@
         <v>4050</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>2016</v>
       </c>
@@ -7973,7 +7965,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>2016</v>
       </c>
@@ -8005,7 +7997,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>2016</v>
       </c>
@@ -8037,7 +8029,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>2016</v>
       </c>
@@ -8069,7 +8061,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>2016</v>
       </c>
@@ -8101,7 +8093,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>2016</v>
       </c>
@@ -8133,7 +8125,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>2016</v>
       </c>
@@ -8165,7 +8157,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>2016</v>
       </c>
@@ -8197,7 +8189,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>2016</v>
       </c>
@@ -8229,7 +8221,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>2016</v>
       </c>
@@ -8261,7 +8253,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>2016</v>
       </c>
@@ -8293,7 +8285,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>2016</v>
       </c>
@@ -8325,7 +8317,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>2016</v>
       </c>
@@ -8357,7 +8349,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>2016</v>
       </c>
@@ -8389,7 +8381,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>2016</v>
       </c>
@@ -8421,7 +8413,7 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>2016</v>
       </c>
@@ -8453,7 +8445,7 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>2017</v>
       </c>
@@ -8485,7 +8477,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>2017</v>
       </c>
@@ -8517,7 +8509,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>2017</v>
       </c>
@@ -8549,7 +8541,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>2017</v>
       </c>
@@ -8581,7 +8573,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>2017</v>
       </c>
@@ -8613,7 +8605,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>2017</v>
       </c>
@@ -8645,7 +8637,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>2017</v>
       </c>
@@ -8677,7 +8669,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>2017</v>
       </c>
@@ -8709,7 +8701,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>2017</v>
       </c>
@@ -8741,7 +8733,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>2017</v>
       </c>
@@ -8773,7 +8765,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>2017</v>
       </c>
@@ -8805,7 +8797,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>2017</v>
       </c>
@@ -8837,7 +8829,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>2017</v>
       </c>
@@ -8869,7 +8861,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>2017</v>
       </c>
@@ -8901,7 +8893,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>2017</v>
       </c>
@@ -8933,7 +8925,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>2017</v>
       </c>
@@ -8965,7 +8957,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>2018</v>
       </c>
@@ -8997,7 +8989,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>2018</v>
       </c>
@@ -9029,7 +9021,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>2018</v>
       </c>
@@ -9061,7 +9053,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>2018</v>
       </c>
@@ -9093,7 +9085,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>2018</v>
       </c>
@@ -9125,7 +9117,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>2018</v>
       </c>
@@ -9157,7 +9149,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>2018</v>
       </c>
@@ -9189,7 +9181,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>2018</v>
       </c>
@@ -9221,7 +9213,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>2018</v>
       </c>
@@ -9253,7 +9245,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>2018</v>
       </c>
@@ -9285,7 +9277,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>2018</v>
       </c>
@@ -9317,7 +9309,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>2018</v>
       </c>
@@ -9349,7 +9341,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>2018</v>
       </c>
@@ -9381,7 +9373,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>2018</v>
       </c>
@@ -9413,7 +9405,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>2018</v>
       </c>
@@ -9445,7 +9437,7 @@
         <v>3725</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>2018</v>
       </c>
@@ -9477,7 +9469,7 @@
         <v>3725</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>2019</v>
       </c>
@@ -9509,7 +9501,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>2019</v>
       </c>
@@ -9541,7 +9533,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>2019</v>
       </c>
@@ -9573,7 +9565,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>2019</v>
       </c>
@@ -9605,7 +9597,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>2019</v>
       </c>
@@ -9637,7 +9629,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>2019</v>
       </c>
@@ -9669,7 +9661,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>2019</v>
       </c>
@@ -9701,7 +9693,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>2019</v>
       </c>
@@ -9733,7 +9725,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>2019</v>
       </c>
@@ -9765,7 +9757,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>2019</v>
       </c>
@@ -9797,7 +9789,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>2019</v>
       </c>
@@ -9829,7 +9821,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>2019</v>
       </c>
@@ -9861,7 +9853,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>2019</v>
       </c>
@@ -9893,7 +9885,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>2019</v>
       </c>
@@ -9925,7 +9917,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>2019</v>
       </c>
@@ -9957,7 +9949,7 @@
         <v>3889</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>2019</v>
       </c>
@@ -9989,7 +9981,7 @@
         <v>3889</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>2021</v>
       </c>
@@ -10021,7 +10013,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>2021</v>
       </c>
@@ -10053,7 +10045,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>2021</v>
       </c>
@@ -10085,7 +10077,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>2021</v>
       </c>
@@ -10117,7 +10109,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>2021</v>
       </c>
@@ -10149,7 +10141,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>2021</v>
       </c>
@@ -10181,7 +10173,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>2021</v>
       </c>
@@ -10213,7 +10205,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>2021</v>
       </c>
@@ -10245,7 +10237,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>2021</v>
       </c>
@@ -10277,7 +10269,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>2021</v>
       </c>
@@ -10309,7 +10301,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>2021</v>
       </c>
@@ -10341,7 +10333,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>2021</v>
       </c>
@@ -10373,7 +10365,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>2021</v>
       </c>
@@ -10405,7 +10397,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>2021</v>
       </c>
@@ -10437,7 +10429,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>2021</v>
       </c>
@@ -10469,7 +10461,7 @@
         <v>4122</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>2021</v>
       </c>
@@ -10501,7 +10493,7 @@
         <v>4122</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>2022</v>
       </c>
@@ -10533,7 +10525,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>2022</v>
       </c>
@@ -10565,7 +10557,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>2022</v>
       </c>
@@ -10597,7 +10589,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>2022</v>
       </c>
@@ -10629,7 +10621,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>2022</v>
       </c>
@@ -10661,7 +10653,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>2022</v>
       </c>
@@ -10693,7 +10685,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>2022</v>
       </c>
@@ -10725,7 +10717,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>2022</v>
       </c>
@@ -10757,7 +10749,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>2022</v>
       </c>
@@ -10789,7 +10781,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>2022</v>
       </c>
@@ -10821,7 +10813,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>2022</v>
       </c>
@@ -10853,7 +10845,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>2022</v>
       </c>
@@ -10885,7 +10877,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>2022</v>
       </c>
@@ -10917,7 +10909,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>2022</v>
       </c>
@@ -10949,7 +10941,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>2022</v>
       </c>
@@ -10981,7 +10973,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>2022</v>
       </c>
@@ -11026,9 +11018,9 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11063,7 +11055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -11098,7 +11090,7 @@
         <v>0.12444052575082247</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -11133,7 +11125,7 @@
         <v>0.20974200501755216</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -11168,7 +11160,7 @@
         <v>0.29510036433920661</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -11203,7 +11195,7 @@
         <v>0.35342930089946689</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -11238,7 +11230,7 @@
         <v>0.32007287319252836</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -11273,7 +11265,7 @@
         <v>0.37813694492994215</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -11308,7 +11300,7 @@
         <v>0.26830232383423147</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -11356,9 +11348,9 @@
       <selection activeCell="B9" sqref="B9:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -11393,7 +11385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -11428,7 +11420,7 @@
         <v>0.15450697452718384</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -11463,7 +11455,7 @@
         <v>0.28252205722154428</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -11498,7 +11490,7 @@
         <v>0.23811304325360988</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -11533,7 +11525,7 @@
         <v>0.33575397628077447</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -11568,7 +11560,7 @@
         <v>0.28343834490175296</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -11603,7 +11595,7 @@
         <v>0.31736373168392618</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -11638,7 +11630,7 @@
         <v>0.27251220013008454</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -11686,9 +11678,9 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -11723,7 +11715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -11758,7 +11750,7 @@
         <v>0.13930889311283234</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -11793,7 +11785,7 @@
         <v>0.24530082376377477</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -11828,7 +11820,7 @@
         <v>0.26541989777239011</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -11863,7 +11855,7 @@
         <v>0.34440518656670716</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -11898,7 +11890,7 @@
         <v>0.30130634288716446</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -11933,7 +11925,7 @@
         <v>0.34718528670065107</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -11968,7 +11960,7 @@
         <v>0.27073770900711541</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>

</xml_diff>